<commit_message>
Added skills analysis function
Added to bug log for iteration 4

Signed-off-by: jeenyjinjin <43344567+jeenyjinjin@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Metrics/Bug Log.xlsx
+++ b/Metrics/Bug Log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jin\Desktop\IS480 FYP\ChickenDinner\Metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11DA4CC5-DFE5-4FF8-9530-98C336C402DB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4AEAC4-E712-4061-A02F-B733CBC64F96}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5580" activeTab="2" xr2:uid="{15213B53-1A15-41AB-97DA-D24E9FE44667}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Iteration 1" sheetId="1" r:id="rId1"/>
     <sheet name="Iteration 2" sheetId="2" r:id="rId2"/>
     <sheet name="Iteration 3" sheetId="4" r:id="rId3"/>
+    <sheet name="Iteration 4" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t>S/N</t>
   </si>
@@ -113,6 +114,27 @@
   </si>
   <si>
     <t>Upload page</t>
+  </si>
+  <si>
+    <t>Implementing the logout functionality meant edits to UserBean.java were necessary. These changes caused the app to crash during runtime</t>
+  </si>
+  <si>
+    <t>Runtime</t>
+  </si>
+  <si>
+    <t>Skills weightage algorithm not working as expected, returning results inconsistent with expected output</t>
+  </si>
+  <si>
+    <t>Skills analysis</t>
+  </si>
+  <si>
+    <t>critical or high?</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Application crashes when deployed and run on LARC servers</t>
   </si>
 </sst>
 </file>
@@ -179,7 +201,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -242,21 +264,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -282,11 +294,31 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1168,15 +1200,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D144">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="11" priority="2" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D144">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Critical">
+    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="Critical">
       <formula>NOT(ISERROR(SEARCH("Critical",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1189,7 +1221,7 @@
   <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B3" sqref="B3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1475,10 +1507,317 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D63">
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="Low">
+      <formula>NOT(ISERROR(SEARCH("Low",D2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D60">
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="Critical">
+      <formula>NOT(ISERROR(SEARCH("Critical",D2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17DCD191-9D58-4EAD-AA36-ADB59084DF22}">
+  <dimension ref="A1:E63"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="38" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D38" s="2"/>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D39" s="2"/>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D40" s="2"/>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D42" s="2"/>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D44" s="2"/>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D46" s="2"/>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D50" s="2"/>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D53" s="2"/>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D55" s="2"/>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D62" s="2"/>
+    </row>
+    <row r="63" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D63" s="2"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D2:D63">
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="High">
+      <formula>NOT(ISERROR(SEARCH("High",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",D2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>